<commit_message>
Qiu ethan patch 1 (#12)
fn_factory_worker_info 新增回傳 獨立員工列表，職務數字由大排到小。
</commit_message>
<xml_diff>
--- a/foxlink_dispatch/test_data/車間 Layout 座標表_公版_TEST用.xlsx
+++ b/foxlink_dispatch/test_data/車間 Layout 座標表_公版_TEST用.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20383"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32875BE3-0EAD-4FE1-BCFE-69B86E6D3A03}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB3845B-DF21-4160-B962-CFE96DDFAEA3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="36">
   <si>
     <t>rescue</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -119,267 +119,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>d54 e75_event-2-Device_11</t>
-  </si>
-  <si>
-    <t>d54 e75_event-2-Device_12</t>
-  </si>
-  <si>
-    <t>d54 e75_event-2-Device_13</t>
-  </si>
-  <si>
-    <t>n104e75_event-3-Device_1</t>
-  </si>
-  <si>
-    <t>n104e75_event-3-Device_2</t>
-  </si>
-  <si>
-    <t>n104e75_event-3-Device_5</t>
-  </si>
-  <si>
-    <t>n104e75_event-3-Device_6</t>
-  </si>
-  <si>
-    <t>n104e75_event-3-Device_8</t>
-  </si>
-  <si>
-    <t>n104e75_event-3-Device_9</t>
-  </si>
-  <si>
-    <t>n104e75_event-3-Device_10</t>
-  </si>
-  <si>
-    <t>n104e75_event-3-Device_11</t>
-  </si>
-  <si>
-    <t>n104e75_event-3-Device_12</t>
-  </si>
-  <si>
-    <t>n104e75_event-3-Device_13</t>
-  </si>
-  <si>
-    <t>n104e75_event-4-Device_1</t>
-  </si>
-  <si>
-    <t>n104e75_event-4-Device_2</t>
-  </si>
-  <si>
-    <t>n104e75_event-4-Device_5</t>
-  </si>
-  <si>
-    <t>n104e75_event-4-Device_6</t>
-  </si>
-  <si>
-    <t>n104e75_event-4-Device_8</t>
-  </si>
-  <si>
-    <t>n104e75_event-4-Device_9</t>
-  </si>
-  <si>
-    <t>n104e75_event-4-Device_10</t>
-  </si>
-  <si>
-    <t>n104e75_event-4-Device_11</t>
-  </si>
-  <si>
-    <t>n104e75_event-4-Device_12</t>
-  </si>
-  <si>
-    <t>n104e75_event-4-Device_13</t>
-  </si>
-  <si>
-    <t>n84e75_event-1-Device_1</t>
-  </si>
-  <si>
-    <t>n84e75_event-1-Device_2</t>
-  </si>
-  <si>
-    <t>n84e75_event-1-Device_5</t>
-  </si>
-  <si>
-    <t>n84e75_event-1-Device_6</t>
-  </si>
-  <si>
-    <t>n84e75_event-1-Device_7</t>
-  </si>
-  <si>
-    <t>n84e75_event-1-Device_8</t>
-  </si>
-  <si>
-    <t>n84e75_event-1-Device_9</t>
-  </si>
-  <si>
-    <t>n84e75_event-1-Device_10</t>
-  </si>
-  <si>
-    <t>n84e75_event-1-Device_11</t>
-  </si>
-  <si>
-    <t>rescue-workshop_09-1</t>
-  </si>
-  <si>
-    <t>rescue-workshop_09-2</t>
-  </si>
-  <si>
-    <t>rescue-workshop_09-3</t>
-  </si>
-  <si>
-    <t>rescue-workshop_09-4</t>
-  </si>
-  <si>
-    <t>rescue-workshop_09-5</t>
-  </si>
-  <si>
-    <t>rescue-workshop_09-6</t>
-  </si>
-  <si>
-    <t>rescue-workshop_09-7</t>
-  </si>
-  <si>
-    <t>d52 e75_event-1-Device_1</t>
-  </si>
-  <si>
-    <t>d52 e75_event-1-Device_2</t>
-  </si>
-  <si>
-    <t>d52 e75_event-1-Device_5</t>
-  </si>
-  <si>
-    <t>d52 e75_event-1-Device_6</t>
-  </si>
-  <si>
-    <t>d52 e75_event-1-Device_8</t>
-  </si>
-  <si>
-    <t>d52 e75_event-1-Device_9</t>
-  </si>
-  <si>
-    <t>d52 e75_event-1-Device_10</t>
-  </si>
-  <si>
-    <t>d52 e75_event-1-Device_11</t>
-  </si>
-  <si>
-    <t>d52 e75_event-1-Device_12</t>
-  </si>
-  <si>
-    <t>d52 e75_event-1-Device_13</t>
-  </si>
-  <si>
-    <t>d53 e75_event-1-Device_1</t>
-  </si>
-  <si>
-    <t>d53 e75_event-1-Device_2</t>
-  </si>
-  <si>
-    <t>d53 e75_event-1-Device_5</t>
-  </si>
-  <si>
-    <t>d53 e75_event-1-Device_6</t>
-  </si>
-  <si>
-    <t>d53 e75_event-1-Device_8</t>
-  </si>
-  <si>
-    <t>d53 e75_event-1-Device_9</t>
-  </si>
-  <si>
-    <t>d53 e75_event-1-Device_10</t>
-  </si>
-  <si>
-    <t>d53 e75_event-1-Device_11</t>
-  </si>
-  <si>
-    <t>d53 e75_event-1-Device_12</t>
-  </si>
-  <si>
-    <t>d53 e75_event-1-Device_13</t>
-  </si>
-  <si>
-    <t>d53 e75_event-2-Device_1</t>
-  </si>
-  <si>
-    <t>d53 e75_event-2-Device_2</t>
-  </si>
-  <si>
-    <t>d53 e75_event-2-Device_5</t>
-  </si>
-  <si>
-    <t>d53 e75_event-2-Device_6</t>
-  </si>
-  <si>
-    <t>d53 e75_event-2-Device_8</t>
-  </si>
-  <si>
-    <t>d53 e75_event-2-Device_9</t>
-  </si>
-  <si>
-    <t>d53 e75_event-2-Device_10</t>
-  </si>
-  <si>
-    <t>d53 e75_event-2-Device_11</t>
-  </si>
-  <si>
-    <t>d53 e75_event-2-Device_12</t>
-  </si>
-  <si>
-    <t>d53 e75_event-2-Device_13</t>
-  </si>
-  <si>
-    <t>d54 e75_event-1-Device_1</t>
-  </si>
-  <si>
-    <t>d54 e75_event-1-Device_2</t>
-  </si>
-  <si>
-    <t>d54 e75_event-1-Device_5</t>
-  </si>
-  <si>
-    <t>d54 e75_event-1-Device_6</t>
-  </si>
-  <si>
-    <t>d54 e75_event-1-Device_8</t>
-  </si>
-  <si>
-    <t>d54 e75_event-1-Device_9</t>
-  </si>
-  <si>
-    <t>d54 e75_event-1-Device_10</t>
-  </si>
-  <si>
-    <t>d54 e75_event-1-Device_11</t>
-  </si>
-  <si>
-    <t>d54 e75_event-1-Device_12</t>
-  </si>
-  <si>
-    <t>d54 e75_event-1-Device_13</t>
-  </si>
-  <si>
-    <t>d54 e75_event-2-Device_1</t>
-  </si>
-  <si>
-    <t>d54 e75_event-2-Device_2</t>
-  </si>
-  <si>
-    <t>d54 e75_event-2-Device_5</t>
-  </si>
-  <si>
-    <t>d54 e75_event-2-Device_6</t>
-  </si>
-  <si>
-    <t>d54 e75_event-2-Device_8</t>
-  </si>
-  <si>
-    <t>d54 e75_event-2-Device_9</t>
-  </si>
-  <si>
-    <t>d54 e75_event-2-Device_10</t>
-  </si>
-  <si>
-    <t>https://www.adamsmith.haus/python/answers/how-to-check-if-a-string-is-a-url-in-python</t>
-  </si>
-  <si>
     <t>D52</t>
   </si>
   <si>
@@ -417,11 +156,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>https://www.adamsmith.haus/python/answers/how-to-check-if-a-string-is-a-url-in-python</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>sop_link</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.foxlink.com/</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -796,8 +535,8 @@
   <dimension ref="A1:I87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M18" sqref="M18"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K51" sqref="K51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -808,6 +547,7 @@
     <col min="4" max="4" width="14.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="3"/>
     <col min="6" max="6" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -836,21 +576,18 @@
         <v>18</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>122</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>63</v>
-      </c>
       <c r="B2" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>112</v>
+        <v>25</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>120</v>
+        <v>33</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>23</v>
@@ -864,19 +601,16 @@
       <c r="H2" s="2">
         <v>16.399999999999999</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>110</v>
+      <c r="I2" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>64</v>
-      </c>
       <c r="B3" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>112</v>
+        <v>25</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>20</v>
@@ -893,19 +627,16 @@
       <c r="H3" s="2">
         <v>16.399999999999999</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>110</v>
+      <c r="I3" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>65</v>
-      </c>
       <c r="B4" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>111</v>
+        <v>24</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>21</v>
@@ -922,19 +653,16 @@
       <c r="H4" s="2">
         <v>17</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>110</v>
+      <c r="I4" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>66</v>
-      </c>
       <c r="B5" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>111</v>
+        <v>24</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>21</v>
@@ -951,19 +679,16 @@
       <c r="H5" s="2">
         <v>17</v>
       </c>
-      <c r="I5" s="3" t="s">
-        <v>110</v>
+      <c r="I5" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="B6" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>111</v>
+        <v>24</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>21</v>
@@ -980,19 +705,16 @@
       <c r="H6" s="2">
         <v>17</v>
       </c>
-      <c r="I6" s="3" t="s">
-        <v>110</v>
+      <c r="I6" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>68</v>
-      </c>
       <c r="B7" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>111</v>
+        <v>24</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>21</v>
@@ -1009,19 +731,16 @@
       <c r="H7" s="2">
         <v>17</v>
       </c>
-      <c r="I7" s="3" t="s">
-        <v>110</v>
+      <c r="I7" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>69</v>
-      </c>
       <c r="B8" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>111</v>
+        <v>24</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>21</v>
@@ -1038,19 +757,16 @@
       <c r="H8" s="2">
         <v>17</v>
       </c>
-      <c r="I8" s="3" t="s">
-        <v>110</v>
+      <c r="I8" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>70</v>
-      </c>
       <c r="B9" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>111</v>
+        <v>24</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>21</v>
@@ -1067,19 +783,16 @@
       <c r="H9" s="2">
         <v>17</v>
       </c>
-      <c r="I9" s="3" t="s">
-        <v>110</v>
+      <c r="I9" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>71</v>
-      </c>
       <c r="B10" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>111</v>
+        <v>24</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>21</v>
@@ -1096,19 +809,16 @@
       <c r="H10" s="2">
         <v>17</v>
       </c>
-      <c r="I10" s="3" t="s">
-        <v>110</v>
+      <c r="I10" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>72</v>
-      </c>
       <c r="B11" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>111</v>
+        <v>24</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>21</v>
@@ -1125,19 +835,16 @@
       <c r="H11" s="2">
         <v>17</v>
       </c>
-      <c r="I11" s="3" t="s">
-        <v>110</v>
+      <c r="I11" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>73</v>
-      </c>
       <c r="B12" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>115</v>
+        <v>28</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>20</v>
@@ -1154,19 +861,16 @@
       <c r="H12" s="2">
         <v>20.5</v>
       </c>
-      <c r="I12" s="3" t="s">
-        <v>110</v>
+      <c r="I12" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>74</v>
-      </c>
       <c r="B13" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>115</v>
+        <v>28</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>20</v>
@@ -1183,19 +887,16 @@
       <c r="H13" s="2">
         <v>20.5</v>
       </c>
-      <c r="I13" s="3" t="s">
-        <v>110</v>
+      <c r="I13" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>75</v>
-      </c>
       <c r="B14" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>113</v>
+        <v>26</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>21</v>
@@ -1212,19 +913,16 @@
       <c r="H14" s="2">
         <v>23.5</v>
       </c>
-      <c r="I14" s="3" t="s">
-        <v>110</v>
+      <c r="I14" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>76</v>
-      </c>
       <c r="B15" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>113</v>
+        <v>26</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>21</v>
@@ -1241,19 +939,16 @@
       <c r="H15" s="2">
         <v>23.5</v>
       </c>
-      <c r="I15" s="3" t="s">
-        <v>110</v>
+      <c r="I15" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>77</v>
-      </c>
       <c r="B16" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>113</v>
+        <v>26</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>21</v>
@@ -1270,19 +965,16 @@
       <c r="H16" s="2">
         <v>23.5</v>
       </c>
-      <c r="I16" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>78</v>
-      </c>
+      <c r="I16" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>113</v>
+        <v>26</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>21</v>
@@ -1299,19 +991,16 @@
       <c r="H17" s="2">
         <v>23.5</v>
       </c>
-      <c r="I17" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>79</v>
-      </c>
+      <c r="I17" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>113</v>
+        <v>26</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>21</v>
@@ -1328,19 +1017,16 @@
       <c r="H18" s="2">
         <v>23.5</v>
       </c>
-      <c r="I18" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>80</v>
-      </c>
+      <c r="I18" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>113</v>
+        <v>26</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>21</v>
@@ -1357,19 +1043,16 @@
       <c r="H19" s="2">
         <v>23.5</v>
       </c>
-      <c r="I19" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>81</v>
-      </c>
+      <c r="I19" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>113</v>
+        <v>26</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>21</v>
@@ -1386,19 +1069,16 @@
       <c r="H20" s="2">
         <v>23.5</v>
       </c>
-      <c r="I20" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>82</v>
-      </c>
+      <c r="I20" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>113</v>
+        <v>26</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>21</v>
@@ -1415,19 +1095,16 @@
       <c r="H21" s="2">
         <v>23.5</v>
       </c>
-      <c r="I21" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>83</v>
-      </c>
+      <c r="I21" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>113</v>
+        <v>26</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>20</v>
@@ -1444,19 +1121,16 @@
       <c r="H22" s="2">
         <v>18.5</v>
       </c>
-      <c r="I22" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>84</v>
-      </c>
+      <c r="I22" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>113</v>
+        <v>26</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>20</v>
@@ -1473,19 +1147,16 @@
       <c r="H23" s="2">
         <v>18.5</v>
       </c>
-      <c r="I23" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>85</v>
-      </c>
+      <c r="I23" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>113</v>
+        <v>26</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>21</v>
@@ -1502,19 +1173,16 @@
       <c r="H24" s="2">
         <v>20.5</v>
       </c>
-      <c r="I24" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>86</v>
-      </c>
+      <c r="I24" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>113</v>
+        <v>26</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>21</v>
@@ -1531,19 +1199,16 @@
       <c r="H25" s="2">
         <v>20.5</v>
       </c>
-      <c r="I25" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>87</v>
-      </c>
+      <c r="I25" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>113</v>
+        <v>26</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>21</v>
@@ -1560,19 +1225,16 @@
       <c r="H26" s="2">
         <v>20.5</v>
       </c>
-      <c r="I26" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>88</v>
-      </c>
+      <c r="I26" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>113</v>
+        <v>26</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>21</v>
@@ -1589,19 +1251,16 @@
       <c r="H27" s="2">
         <v>20.5</v>
       </c>
-      <c r="I27" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>89</v>
-      </c>
+      <c r="I27" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>113</v>
+        <v>26</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>21</v>
@@ -1618,19 +1277,16 @@
       <c r="H28" s="2">
         <v>20.5</v>
       </c>
-      <c r="I28" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>90</v>
-      </c>
+      <c r="I28" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>113</v>
+        <v>26</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>21</v>
@@ -1648,18 +1304,15 @@
         <v>20.5</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>91</v>
-      </c>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>113</v>
+        <v>26</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>21</v>
@@ -1676,19 +1329,16 @@
       <c r="H30" s="2">
         <v>20.5</v>
       </c>
-      <c r="I30" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>92</v>
-      </c>
+      <c r="I30" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>113</v>
+        <v>26</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>21</v>
@@ -1705,19 +1355,16 @@
       <c r="H31" s="2">
         <v>20.5</v>
       </c>
-      <c r="I31" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>93</v>
-      </c>
+      <c r="I31" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>116</v>
+        <v>29</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>20</v>
@@ -1734,19 +1381,16 @@
       <c r="H32" s="2">
         <v>14</v>
       </c>
-      <c r="I32" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>94</v>
-      </c>
+      <c r="I32" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>116</v>
+        <v>29</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>20</v>
@@ -1763,19 +1407,16 @@
       <c r="H33" s="2">
         <v>14</v>
       </c>
-      <c r="I33" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>95</v>
-      </c>
+      <c r="I33" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>114</v>
+        <v>27</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>21</v>
@@ -1792,22 +1433,19 @@
       <c r="H34" s="2">
         <v>14.2</v>
       </c>
-      <c r="I34" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>96</v>
-      </c>
+      <c r="I34" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>114</v>
+        <v>27</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>119</v>
+        <v>32</v>
       </c>
       <c r="E35" s="3">
         <v>1</v>
@@ -1821,19 +1459,16 @@
       <c r="H35" s="2">
         <v>14.2</v>
       </c>
-      <c r="I35" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>97</v>
-      </c>
+      <c r="I35" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>114</v>
+        <v>27</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>21</v>
@@ -1850,19 +1485,16 @@
       <c r="H36" s="2">
         <v>14.2</v>
       </c>
-      <c r="I36" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>98</v>
-      </c>
+      <c r="I36" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>114</v>
+        <v>27</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>21</v>
@@ -1879,19 +1511,16 @@
       <c r="H37" s="2">
         <v>14.2</v>
       </c>
-      <c r="I37" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>99</v>
-      </c>
+      <c r="I37" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>114</v>
+        <v>27</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>21</v>
@@ -1908,19 +1537,16 @@
       <c r="H38" s="2">
         <v>14.2</v>
       </c>
-      <c r="I38" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>100</v>
-      </c>
+      <c r="I38" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>114</v>
+        <v>27</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>21</v>
@@ -1937,19 +1563,16 @@
       <c r="H39" s="2">
         <v>14.2</v>
       </c>
-      <c r="I39" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>101</v>
-      </c>
+      <c r="I39" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>114</v>
+        <v>27</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>21</v>
@@ -1966,19 +1589,16 @@
       <c r="H40" s="2">
         <v>14.2</v>
       </c>
-      <c r="I40" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
-        <v>102</v>
-      </c>
+      <c r="I40" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>114</v>
+        <v>27</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>21</v>
@@ -1995,19 +1615,16 @@
       <c r="H41" s="2">
         <v>14.2</v>
       </c>
-      <c r="I41" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>103</v>
-      </c>
+      <c r="I41" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>114</v>
+        <v>27</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>20</v>
@@ -2024,19 +1641,16 @@
       <c r="H42" s="2">
         <v>11.2</v>
       </c>
-      <c r="I42" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
-        <v>104</v>
-      </c>
+      <c r="I42" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B43" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>114</v>
+        <v>27</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>20</v>
@@ -2053,19 +1667,16 @@
       <c r="H43" s="2">
         <v>11.2</v>
       </c>
-      <c r="I43" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
-        <v>105</v>
-      </c>
+      <c r="I43" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B44" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>114</v>
+        <v>27</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>21</v>
@@ -2082,19 +1693,16 @@
       <c r="H44" s="2">
         <v>11.4</v>
       </c>
-      <c r="I44" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
-        <v>106</v>
-      </c>
+      <c r="I44" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B45" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>114</v>
+        <v>27</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>21</v>
@@ -2111,19 +1719,16 @@
       <c r="H45" s="2">
         <v>11.4</v>
       </c>
-      <c r="I45" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
-        <v>107</v>
-      </c>
+      <c r="I45" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B46" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>114</v>
+        <v>27</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>21</v>
@@ -2140,19 +1745,16 @@
       <c r="H46" s="2">
         <v>11.4</v>
       </c>
-      <c r="I46" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
-        <v>108</v>
-      </c>
+      <c r="I46" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B47" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>114</v>
+        <v>27</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>21</v>
@@ -2169,19 +1771,16 @@
       <c r="H47" s="2">
         <v>11.4</v>
       </c>
-      <c r="I47" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
-        <v>109</v>
-      </c>
+      <c r="I47" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B48" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>114</v>
+        <v>27</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>21</v>
@@ -2198,19 +1797,16 @@
       <c r="H48" s="2">
         <v>11.4</v>
       </c>
-      <c r="I48" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="I48" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>114</v>
+        <v>27</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>21</v>
@@ -2227,19 +1823,16 @@
       <c r="H49" s="2">
         <v>11.4</v>
       </c>
-      <c r="I49" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="I49" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>114</v>
+        <v>27</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>21</v>
@@ -2256,19 +1849,16 @@
       <c r="H50" s="2">
         <v>11.4</v>
       </c>
-      <c r="I50" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
-        <v>26</v>
-      </c>
+      <c r="I50" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>114</v>
+        <v>27</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>21</v>
@@ -2285,19 +1875,16 @@
       <c r="H51" s="2">
         <v>11.4</v>
       </c>
-      <c r="I51" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
-        <v>27</v>
-      </c>
+      <c r="I51" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B52" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>117</v>
+        <v>30</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>20</v>
@@ -2314,19 +1901,16 @@
       <c r="H52" s="2">
         <v>8.4</v>
       </c>
-      <c r="I52" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
-        <v>28</v>
-      </c>
+      <c r="I52" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B53" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>117</v>
+        <v>30</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>20</v>
@@ -2343,19 +1927,16 @@
       <c r="H53" s="2">
         <v>8.4</v>
       </c>
-      <c r="I53" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
-        <v>29</v>
-      </c>
+      <c r="I53" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B54" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>117</v>
+        <v>30</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>21</v>
@@ -2372,19 +1953,16 @@
       <c r="H54" s="2">
         <v>8.4</v>
       </c>
-      <c r="I54" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
+      <c r="I54" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B55" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C55" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>117</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>21</v>
@@ -2401,19 +1979,16 @@
       <c r="H55" s="2">
         <v>8.4</v>
       </c>
-      <c r="I55" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
-        <v>31</v>
-      </c>
+      <c r="I55" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B56" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>117</v>
+        <v>30</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>21</v>
@@ -2430,19 +2005,16 @@
       <c r="H56" s="2">
         <v>8.4</v>
       </c>
-      <c r="I56" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="3" t="s">
-        <v>32</v>
-      </c>
+      <c r="I56" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B57" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>117</v>
+        <v>30</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>21</v>
@@ -2459,19 +2031,16 @@
       <c r="H57" s="2">
         <v>8.4</v>
       </c>
-      <c r="I57" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="3" t="s">
-        <v>33</v>
-      </c>
+      <c r="I57" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B58" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>117</v>
+        <v>30</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>21</v>
@@ -2488,19 +2057,16 @@
       <c r="H58" s="2">
         <v>8.4</v>
       </c>
-      <c r="I58" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="3" t="s">
-        <v>34</v>
-      </c>
+      <c r="I58" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B59" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>117</v>
+        <v>30</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>21</v>
@@ -2517,19 +2083,16 @@
       <c r="H59" s="2">
         <v>8.4</v>
       </c>
-      <c r="I59" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="3" t="s">
-        <v>35</v>
-      </c>
+      <c r="I59" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B60" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>117</v>
+        <v>30</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>21</v>
@@ -2546,19 +2109,16 @@
       <c r="H60" s="2">
         <v>8.4</v>
       </c>
-      <c r="I60" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="3" t="s">
-        <v>36</v>
-      </c>
+      <c r="I60" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B61" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>117</v>
+        <v>30</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>21</v>
@@ -2575,19 +2135,16 @@
       <c r="H61" s="2">
         <v>8.4</v>
       </c>
-      <c r="I61" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="3" t="s">
-        <v>37</v>
-      </c>
+      <c r="I61" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B62" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>117</v>
+        <v>30</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>20</v>
@@ -2604,19 +2161,16 @@
       <c r="H62" s="2">
         <v>5.6</v>
       </c>
-      <c r="I62" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="3" t="s">
-        <v>38</v>
-      </c>
+      <c r="I62" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B63" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>117</v>
+        <v>30</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>20</v>
@@ -2633,19 +2187,16 @@
       <c r="H63" s="2">
         <v>5.6</v>
       </c>
-      <c r="I63" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="3" t="s">
-        <v>39</v>
-      </c>
+      <c r="I63" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B64" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>117</v>
+        <v>30</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>21</v>
@@ -2662,19 +2213,16 @@
       <c r="H64" s="2">
         <v>5.8</v>
       </c>
-      <c r="I64" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="I64" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B65" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>117</v>
+        <v>30</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>21</v>
@@ -2691,22 +2239,19 @@
       <c r="H65" s="2">
         <v>5.8</v>
       </c>
-      <c r="I65" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" s="3" t="s">
-        <v>41</v>
-      </c>
+      <c r="I65" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B66" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>117</v>
+        <v>30</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>119</v>
+        <v>32</v>
       </c>
       <c r="E66" s="3">
         <v>4</v>
@@ -2720,19 +2265,16 @@
       <c r="H66" s="2">
         <v>5.8</v>
       </c>
-      <c r="I66" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="I66" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B67" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>117</v>
+        <v>30</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>21</v>
@@ -2749,19 +2291,16 @@
       <c r="H67" s="2">
         <v>5.8</v>
       </c>
-      <c r="I67" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" s="3" t="s">
-        <v>43</v>
-      </c>
+      <c r="I67" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B68" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>117</v>
+        <v>30</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>21</v>
@@ -2778,19 +2317,16 @@
       <c r="H68" s="2">
         <v>5.8</v>
       </c>
-      <c r="I68" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" s="3" t="s">
-        <v>44</v>
-      </c>
+      <c r="I68" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B69" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>117</v>
+        <v>30</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>21</v>
@@ -2807,19 +2343,16 @@
       <c r="H69" s="2">
         <v>5.8</v>
       </c>
-      <c r="I69" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="I69" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B70" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>117</v>
+        <v>30</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>21</v>
@@ -2836,19 +2369,16 @@
       <c r="H70" s="2">
         <v>5.8</v>
       </c>
-      <c r="I70" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="I70" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B71" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>117</v>
+        <v>30</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>21</v>
@@ -2865,19 +2395,16 @@
       <c r="H71" s="2">
         <v>5.8</v>
       </c>
-      <c r="I71" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A72" s="3" t="s">
-        <v>47</v>
-      </c>
+      <c r="I71" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B72" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>118</v>
+        <v>31</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>20</v>
@@ -2894,19 +2421,16 @@
       <c r="H72" s="2">
         <v>2.8</v>
       </c>
-      <c r="I72" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A73" s="3" t="s">
-        <v>48</v>
-      </c>
+      <c r="I72" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B73" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>118</v>
+        <v>31</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>20</v>
@@ -2923,19 +2447,16 @@
       <c r="H73" s="2">
         <v>2.8</v>
       </c>
-      <c r="I73" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A74" s="3" t="s">
-        <v>49</v>
-      </c>
+      <c r="I73" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B74" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>118</v>
+        <v>31</v>
       </c>
       <c r="D74" s="3" t="s">
         <v>21</v>
@@ -2952,19 +2473,16 @@
       <c r="H74" s="2">
         <v>3</v>
       </c>
-      <c r="I74" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A75" s="3" t="s">
-        <v>50</v>
-      </c>
+      <c r="I74" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B75" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>118</v>
+        <v>31</v>
       </c>
       <c r="D75" s="3" t="s">
         <v>21</v>
@@ -2981,19 +2499,16 @@
       <c r="H75" s="2">
         <v>3</v>
       </c>
-      <c r="I75" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A76" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="I75" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B76" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>118</v>
+        <v>31</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>21</v>
@@ -3010,19 +2525,16 @@
       <c r="H76" s="2">
         <v>3</v>
       </c>
-      <c r="I76" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A77" s="3" t="s">
-        <v>52</v>
-      </c>
+      <c r="I76" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B77" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>118</v>
+        <v>31</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>21</v>
@@ -3039,19 +2551,16 @@
       <c r="H77" s="2">
         <v>3</v>
       </c>
-      <c r="I77" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A78" s="3" t="s">
-        <v>53</v>
-      </c>
+      <c r="I77" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B78" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>118</v>
+        <v>31</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>21</v>
@@ -3068,19 +2577,16 @@
       <c r="H78" s="2">
         <v>3</v>
       </c>
-      <c r="I78" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A79" s="3" t="s">
-        <v>54</v>
-      </c>
+      <c r="I78" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B79" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>118</v>
+        <v>31</v>
       </c>
       <c r="D79" s="3" t="s">
         <v>21</v>
@@ -3097,19 +2603,16 @@
       <c r="H79" s="2">
         <v>3</v>
       </c>
-      <c r="I79" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A80" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="I79" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B80" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>118</v>
+        <v>31</v>
       </c>
       <c r="D80" s="3" t="s">
         <v>21</v>
@@ -3126,14 +2629,11 @@
       <c r="H80" s="2">
         <v>3</v>
       </c>
-      <c r="I80" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A81" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="I80" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B81" s="3" t="s">
         <v>19</v>
       </c>
@@ -3151,10 +2651,7 @@
       </c>
       <c r="I81" s="3"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A82" s="3" t="s">
-        <v>57</v>
-      </c>
+    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B82" s="3" t="s">
         <v>19</v>
       </c>
@@ -3172,10 +2669,7 @@
       </c>
       <c r="I82" s="3"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A83" s="3" t="s">
-        <v>58</v>
-      </c>
+    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B83" s="3" t="s">
         <v>19</v>
       </c>
@@ -3193,10 +2687,7 @@
       </c>
       <c r="I83" s="3"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A84" s="3" t="s">
-        <v>59</v>
-      </c>
+    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B84" s="3" t="s">
         <v>19</v>
       </c>
@@ -3214,10 +2705,7 @@
       </c>
       <c r="I84" s="3"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A85" s="3" t="s">
-        <v>60</v>
-      </c>
+    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B85" s="3" t="s">
         <v>19</v>
       </c>
@@ -3235,10 +2723,7 @@
       </c>
       <c r="I85" s="3"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A86" s="3" t="s">
-        <v>61</v>
-      </c>
+    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B86" s="3" t="s">
         <v>19</v>
       </c>
@@ -3256,10 +2741,7 @@
       </c>
       <c r="I86" s="3"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A87" s="3" t="s">
-        <v>62</v>
-      </c>
+    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B87" s="3" t="s">
         <v>19</v>
       </c>
@@ -3281,10 +2763,11 @@
   <sheetProtection insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="I29" r:id="rId1" xr:uid="{1B5554B7-2B32-4A70-AE26-CA24A62645D7}"/>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{254D3340-CC90-46A3-8432-93169BD632AE}"/>
+    <hyperlink ref="I3:I80" r:id="rId2" display="https://www.foxlink.com/" xr:uid="{EDC9DFDA-03B4-412B-84B8-FC9183133DD9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
   <ignoredErrors>
     <ignoredError sqref="E2" numberStoredAsText="1"/>
   </ignoredErrors>

</xml_diff>